<commit_message>
Update rule set to include 2 week average BPRE
</commit_message>
<xml_diff>
--- a/src/player_simulation.xlsx
+++ b/src/player_simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33441D43-83C6-EE46-A927-810B8DEF3EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E62CA-6C07-5546-AC01-EB228C40CBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="2020" windowWidth="33920" windowHeight="18340" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="31620" yWindow="2080" windowWidth="33860" windowHeight="18340" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -1072,25 +1072,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1841C9-D21C-2040-9467-2F510B1F6134}">
-  <dimension ref="A1:AL785"/>
+  <dimension ref="A1:AN785"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="10.83203125" customWidth="1"/>
-    <col min="13" max="27" width="10.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="15.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="34" width="10.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="27" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="15.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="34" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="10.83203125" collapsed="1"/>
     <col min="36" max="38" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:40" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>33</v>
       </c>
@@ -1198,7 +1199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1281,15 +1282,18 @@
         <v>0</v>
       </c>
       <c r="AJ2" s="2">
-        <f>SUM(R2:V2,Y2:AA2,AE2)</f>
+        <f t="shared" ref="AJ2:AJ23" si="0">SUM(R2:V2,Y2:AA2,AE2)</f>
         <v>68</v>
       </c>
       <c r="AL2" s="2">
-        <f>AJ2-F2</f>
+        <f t="shared" ref="AL2:AL23" si="1">AJ2-F2</f>
         <v>32.379562043795623</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+      <c r="AN2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1304,7 +1308,7 @@
         <v>517000</v>
       </c>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F23" si="0">E3/13700</f>
+        <f t="shared" ref="F3:F23" si="2">E3/13700</f>
         <v>37.737226277372265</v>
       </c>
       <c r="H3" s="4">
@@ -1377,16 +1381,18 @@
       </c>
       <c r="AH3" s="2"/>
       <c r="AJ3" s="2">
-        <f>SUM(R3:V3,Y3:AA3,AE3)</f>
+        <f t="shared" si="0"/>
         <v>42.3</v>
       </c>
       <c r="AK3"/>
       <c r="AL3" s="2">
-        <f>AJ3-F3</f>
-        <v>4.5627737226277318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="AN3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <f>A3+1</f>
         <v>3</v>
@@ -1402,7 +1408,7 @@
         <v>539000</v>
       </c>
       <c r="F4" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>39.34306569343066</v>
       </c>
       <c r="H4" s="4">
@@ -1475,18 +1481,21 @@
       </c>
       <c r="AH4" s="2"/>
       <c r="AJ4" s="2">
-        <f>SUM(R4:V4,Y4:AA4,AE4)</f>
+        <f t="shared" si="0"/>
         <v>56.6</v>
       </c>
       <c r="AK4"/>
       <c r="AL4" s="2">
-        <f>AJ4-F4</f>
+        <f t="shared" si="1"/>
         <v>17.256934306569342</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+      <c r="AN4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <f t="shared" ref="A5:A23" si="1">A4+1</f>
+        <f t="shared" ref="A5:A23" si="3">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1500,7 +1509,7 @@
         <v>565000</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41.240875912408761</v>
       </c>
       <c r="H5" s="4">
@@ -1573,18 +1582,18 @@
       </c>
       <c r="AH5" s="2"/>
       <c r="AJ5" s="2">
-        <f>SUM(R5:V5,Y5:AA5,AE5)</f>
+        <f t="shared" si="0"/>
         <v>55.7</v>
       </c>
       <c r="AK5"/>
       <c r="AL5" s="2">
-        <f>AJ5-F5</f>
+        <f t="shared" si="1"/>
         <v>14.459124087591242</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -1598,7 +1607,7 @@
         <v>586000</v>
       </c>
       <c r="F6" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>42.773722627737229</v>
       </c>
       <c r="H6" s="4">
@@ -1671,18 +1680,18 @@
       </c>
       <c r="AH6" s="2"/>
       <c r="AJ6" s="2">
-        <f>SUM(R6:V6,Y6:AA6,AE6)</f>
+        <f t="shared" si="0"/>
         <v>59.7</v>
       </c>
       <c r="AK6"/>
       <c r="AL6" s="2">
-        <f>AJ6-F6</f>
+        <f t="shared" si="1"/>
         <v>16.926277372262774</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -1696,7 +1705,7 @@
         <v>617000</v>
       </c>
       <c r="F7" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>45.036496350364963</v>
       </c>
       <c r="H7" s="4">
@@ -1769,18 +1778,18 @@
       </c>
       <c r="AH7" s="2"/>
       <c r="AJ7" s="2">
-        <f>SUM(R7:V7,Y7:AA7,AE7)</f>
+        <f t="shared" si="0"/>
         <v>50.3</v>
       </c>
       <c r="AK7"/>
       <c r="AL7" s="2">
-        <f>AJ7-F7</f>
+        <f t="shared" si="1"/>
         <v>5.2635036496350338</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1794,7 +1803,7 @@
         <v>640000</v>
       </c>
       <c r="F8" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46.715328467153284</v>
       </c>
       <c r="H8" s="4">
@@ -1867,18 +1876,18 @@
       </c>
       <c r="AH8" s="2"/>
       <c r="AJ8" s="2">
-        <f>SUM(R8:V8,Y8:AA8,AE8)</f>
+        <f t="shared" si="0"/>
         <v>71.2</v>
       </c>
       <c r="AK8"/>
       <c r="AL8" s="2">
-        <f>AJ8-F8</f>
+        <f t="shared" si="1"/>
         <v>24.484671532846718</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -1892,7 +1901,7 @@
         <v>688000</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>50.21897810218978</v>
       </c>
       <c r="H9" s="4">
@@ -1965,18 +1974,18 @@
       </c>
       <c r="AH9" s="2"/>
       <c r="AJ9" s="2">
-        <f>SUM(R9:V9,Y9:AA9,AE9)</f>
+        <f t="shared" si="0"/>
         <v>36.6</v>
       </c>
       <c r="AK9"/>
       <c r="AL9" s="2">
-        <f>AJ9-F9</f>
+        <f t="shared" si="1"/>
         <v>-13.618978102189779</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -1990,7 +1999,7 @@
         <v>701000</v>
       </c>
       <c r="F10" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>51.167883211678834</v>
       </c>
       <c r="H10" s="4">
@@ -2063,18 +2072,18 @@
       </c>
       <c r="AH10" s="2"/>
       <c r="AJ10" s="2">
-        <f>SUM(R10:V10,Y10:AA10,AE10)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="AK10"/>
       <c r="AL10" s="2">
-        <f>AJ10-F10</f>
+        <f t="shared" si="1"/>
         <v>5.8321167883211658</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -2088,7 +2097,7 @@
         <v>713000</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52.043795620437955</v>
       </c>
       <c r="H11" s="4">
@@ -2161,18 +2170,18 @@
       </c>
       <c r="AH11" s="2"/>
       <c r="AJ11" s="2">
-        <f>SUM(R11:V11,Y11:AA11,AE11)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="AK11"/>
       <c r="AL11" s="2">
-        <f>AJ11-F11</f>
+        <f t="shared" si="1"/>
         <v>-7.0437956204379546</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -2186,7 +2195,7 @@
         <v>705000</v>
       </c>
       <c r="F12" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>51.459854014598541</v>
       </c>
       <c r="H12" s="4">
@@ -2259,18 +2268,18 @@
       </c>
       <c r="AH12" s="2"/>
       <c r="AJ12" s="2">
-        <f>SUM(R12:V12,Y12:AA12,AE12)</f>
+        <f t="shared" si="0"/>
         <v>63.1</v>
       </c>
       <c r="AK12"/>
       <c r="AL12" s="2">
-        <f>AJ12-F12</f>
+        <f t="shared" si="1"/>
         <v>11.64014598540146</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -2284,7 +2293,7 @@
         <v>697000</v>
       </c>
       <c r="F13" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>50.875912408759127</v>
       </c>
       <c r="H13" s="4">
@@ -2357,18 +2366,18 @@
       </c>
       <c r="AH13" s="2"/>
       <c r="AJ13" s="2">
-        <f>SUM(R13:V13,Y13:AA13,AE13)</f>
+        <f t="shared" si="0"/>
         <v>58.3</v>
       </c>
       <c r="AK13"/>
       <c r="AL13" s="2">
-        <f>AJ13-F13</f>
+        <f t="shared" si="1"/>
         <v>7.4240875912408697</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -2381,7 +2390,7 @@
         <v>693000</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>50.583941605839414</v>
       </c>
       <c r="H14" s="4">
@@ -2435,18 +2444,18 @@
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AJ14" s="2">
-        <f>SUM(R14:V14,Y14:AA14,AE14)</f>
+        <f t="shared" si="0"/>
         <v>73.900000000000006</v>
       </c>
       <c r="AK14"/>
       <c r="AL14" s="2">
-        <f>AJ14-F14</f>
+        <f t="shared" si="1"/>
         <v>23.316058394160592</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -2459,7 +2468,7 @@
         <v>731000</v>
       </c>
       <c r="F15" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>53.357664233576642</v>
       </c>
       <c r="H15" s="4">
@@ -2513,18 +2522,18 @@
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AJ15" s="2">
-        <f>SUM(R15:V15,Y15:AA15,AE15)</f>
+        <f t="shared" si="0"/>
         <v>57.9</v>
       </c>
       <c r="AK15"/>
       <c r="AL15" s="2">
-        <f>AJ15-F15</f>
+        <f t="shared" si="1"/>
         <v>4.5423357664233563</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -2537,7 +2546,7 @@
         <v>749000</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54.67153284671533</v>
       </c>
       <c r="H16" s="4">
@@ -2591,18 +2600,18 @@
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AJ16" s="2">
-        <f>SUM(R16:V16,Y16:AA16,AE16)</f>
+        <f t="shared" si="0"/>
         <v>42.2</v>
       </c>
       <c r="AK16"/>
       <c r="AL16" s="2">
-        <f>AJ16-F16</f>
+        <f t="shared" si="1"/>
         <v>-12.471532846715327</v>
       </c>
     </row>
     <row r="17" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -2615,7 +2624,7 @@
         <v>740000</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54.014598540145982</v>
       </c>
       <c r="H17" s="4">
@@ -2669,18 +2678,18 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AJ17" s="2">
-        <f>SUM(R17:V17,Y17:AA17,AE17)</f>
+        <f t="shared" si="0"/>
         <v>72.099999999999994</v>
       </c>
       <c r="AK17"/>
       <c r="AL17" s="2">
-        <f>AJ17-F17</f>
+        <f t="shared" si="1"/>
         <v>18.085401459854012</v>
       </c>
     </row>
     <row r="18" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -2693,7 +2702,7 @@
         <v>744000</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54.306569343065696</v>
       </c>
       <c r="H18" s="4">
@@ -2747,18 +2756,18 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AJ18" s="2">
-        <f>SUM(R18:V18,Y18:AA18,AE18)</f>
+        <f t="shared" si="0"/>
         <v>67.7</v>
       </c>
       <c r="AK18"/>
       <c r="AL18" s="2">
-        <f>AJ18-F18</f>
+        <f t="shared" si="1"/>
         <v>13.393430656934306</v>
       </c>
     </row>
     <row r="19" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -2771,7 +2780,7 @@
         <v>745000</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54.379562043795623</v>
       </c>
       <c r="H19" s="4">
@@ -2825,18 +2834,18 @@
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AJ19" s="2">
-        <f>SUM(R19:V19,Y19:AA19,AE19)</f>
+        <f t="shared" si="0"/>
         <v>82.4</v>
       </c>
       <c r="AK19"/>
       <c r="AL19" s="2">
-        <f>AJ19-F19</f>
+        <f t="shared" si="1"/>
         <v>28.020437956204383</v>
       </c>
     </row>
     <row r="20" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
@@ -2849,7 +2858,7 @@
         <v>761000</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>55.54744525547445</v>
       </c>
       <c r="H20" s="4">
@@ -2903,18 +2912,18 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AJ20" s="2">
-        <f>SUM(R20:V20,Y20:AA20,AE20)</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="AK20"/>
       <c r="AL20" s="2">
-        <f>AJ20-F20</f>
+        <f t="shared" si="1"/>
         <v>7.4525547445255498</v>
       </c>
     </row>
     <row r="21" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -2927,7 +2936,7 @@
         <v>771000</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>56.277372262773724</v>
       </c>
       <c r="H21" s="4">
@@ -2981,18 +2990,18 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AJ21" s="2">
-        <f>SUM(R21:V21,Y21:AA21,AE21)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="AK21"/>
       <c r="AL21" s="2">
-        <f>AJ21-F21</f>
+        <f t="shared" si="1"/>
         <v>3.7226277372262757</v>
       </c>
     </row>
     <row r="22" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
@@ -3005,7 +3014,7 @@
         <v>780000</v>
       </c>
       <c r="F22" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>56.934306569343065</v>
       </c>
       <c r="H22" s="4">
@@ -3059,18 +3068,18 @@
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AJ22" s="2">
-        <f>SUM(R22:V22,Y22:AA22,AE22)</f>
+        <f t="shared" si="0"/>
         <v>62.8</v>
       </c>
       <c r="AK22"/>
       <c r="AL22" s="2">
-        <f>AJ22-F22</f>
+        <f t="shared" si="1"/>
         <v>5.8656934306569326</v>
       </c>
     </row>
     <row r="23" spans="1:38" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -3083,7 +3092,7 @@
         <v>779000</v>
       </c>
       <c r="F23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>56.861313868613138</v>
       </c>
       <c r="H23" s="4">
@@ -3136,12 +3145,12 @@
       </c>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2">
-        <f>SUM(R23:V23,Y23:AA23,AE23)</f>
+        <f t="shared" si="0"/>
         <v>37.299999999999997</v>
       </c>
       <c r="AK23"/>
       <c r="AL23" s="2">
-        <f>AJ23-F23</f>
+        <f t="shared" si="1"/>
         <v>-19.561313868613141</v>
       </c>
     </row>

</xml_diff>